<commit_message>
Adiciona arquivo de dados e atualiza lógica de envio de e-mails com informações de vencimento
</commit_message>
<xml_diff>
--- a/clientes_cbpce.xlsx
+++ b/clientes_cbpce.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breri\Documents\Python\automacao-email\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A75E55A-5E2D-46C3-812A-DEF6D475F338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="360" yWindow="2985" windowWidth="13980" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -50,18 +56,18 @@
     <t>br.ericktk@gmail.com</t>
   </si>
   <si>
-    <t>faturas/Berick Boleto Jun25</t>
+    <t>faturas/Bruno Erick Jun25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;R$ &quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,15 +137,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -212,6 +218,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -393,14 +407,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
@@ -410,7 +424,7 @@
     <col min="6" max="6" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,11 +444,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
@@ -450,73 +464,73 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
+      <c r="C3" s="8"/>
       <c r="D3" s="1"/>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5" s="2"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D6" s="1"/>
       <c r="E6" s="2"/>
       <c r="F6" s="3"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7">
-      <c r="C7" s="7"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D7" s="1"/>
       <c r="E7" s="2"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D8" s="1"/>
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
       <c r="E9" s="2"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
       <c r="E10" s="2"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
       <c r="F14" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -524,12 +538,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -537,12 +551,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>